<commit_message>
bug fixed and some new functions
</commit_message>
<xml_diff>
--- a/cmdcount.xlsx
+++ b/cmdcount.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>160</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2">
@@ -438,7 +438,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
pick and daily --> google sheets
</commit_message>
<xml_diff>
--- a/cmdcount.xlsx
+++ b/cmdcount.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">

</xml_diff>